<commit_message>
Guion editado y con corrección de estilo
Hay también una versión actualizada de la solicitud gráfica.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/SolicitudGrafica CN_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/SolicitudGrafica CN_09_01_CO.xlsx
@@ -16,12 +16,12 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="226">
   <si>
     <t>Fecha:</t>
   </si>
@@ -612,17 +612,6 @@
     <t>Diagrama de los procesos de replicación, traducción y transcripción</t>
   </si>
   <si>
-    <t xml:space="preserve">La imagen es para ilustrar. Eliminar de la imagen los textos que se encuentran en color rojo.
-Escribir los demás nombres en español, así:
-replicación (ADN – ADN)
-ADN
-transcripción (ADN -&gt; ARN)
-ARN
-traducción (ARN -&gt; Proteína)
-Proteína
-</t>
-  </si>
-  <si>
     <t>Fotografía</t>
   </si>
   <si>
@@ -647,9 +636,6 @@
     <t>https://upload.wikimedia.org/wikipedia/commons/thumb/3/37/Difference_DNA_RNA-EN.svg/1280px-Difference_DNA_RNA-EN.svg.png</t>
   </si>
   <si>
-    <t>Comparación del ARN ocn el ADN</t>
-  </si>
-  <si>
     <t xml:space="preserve">http://es.dreamstime.com/imagen-de-archivo-amino%C3%A1cidos-as-estructuras-qu%C3%ADmicas-del-comm-image30574281  </t>
   </si>
   <si>
@@ -662,9 +648,6 @@
     <t>http://www.genomasur.com/BCH/BCH_libro/capitulo_02.htm</t>
   </si>
   <si>
-    <t>Niveles estructurales de una proteína</t>
-  </si>
-  <si>
     <t>Ilustrar</t>
   </si>
   <si>
@@ -696,6 +679,27 @@
   </si>
   <si>
     <t>Diagrama que representa la regulación génica</t>
+  </si>
+  <si>
+    <t>La imagen es para ilustrar. Eliminar de la imagen los textos que se encuentran en color rojo. Escribir los demás nombres en español, así: replicación (ADN – ADN), ADN, transcripción (ADN -&gt; ARN), ARN, traducción (ARN -&gt; Proteína), Proteína</t>
+  </si>
+  <si>
+    <t>Si entiendo bien, esta imagen requiere que se cite. ¿Nos sirve? No se consiguen fotos sin esas exigencias: si no se puede usar, habrá que eliminarla.</t>
+  </si>
+  <si>
+    <t>Comparación del ARN con el ADN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traducir los términos: Cytosine = Citosina; Guanine = Guanina; Adenine = Adenina; Uracil = Uracilo; Nucleobases of RNA = Nucleótidos del ARN; Nucleobases = Nucleótidos; Base pair = Par de bases; RNA Ribonucleic acid = ARN Ácido ribonucleico; DNA Deoxyribonucleic acid = ADN Ácido desoxiribonucléico; Thymine = Timina; Nucleobases of DNA = ADN nucleótidos del ADN. La parte que dice Helix of sugar-phosphates debe ser eliminada. </t>
+  </si>
+  <si>
+    <t>Niveles estructurales de las proteínas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilustrar. Escribir en cada imagen, de arriba hacia abajo, "Estructura primaria", "Estructura secundaria", "Estructura terciaria" y "Estructura cuaternaria". Así, estructura primaria corresponde a "Aminoácidos", y Estructura cuaternaria aparece en donde dice "Subunidad". </t>
+  </si>
+  <si>
+    <t>Ilustrar. Eliminar el recuadro verde que aparece en la parte superior de la imagen, y todo su contenido.</t>
   </si>
 </sst>
 </file>
@@ -1645,6 +1649,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1743,10 +1751,6 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2589,9 +2593,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2637,14 +2641,14 @@
       <c r="B2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="F2" s="79" t="s">
+      <c r="D2" s="89"/>
+      <c r="F2" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="80"/>
+      <c r="G2" s="82"/>
       <c r="H2" s="58"/>
       <c r="I2" s="58"/>
       <c r="J2" s="14"/>
@@ -2668,14 +2672,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="88">
+      <c r="C3" s="90">
         <v>9</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="F3" s="81">
+      <c r="D3" s="91"/>
+      <c r="F3" s="83">
         <v>42221</v>
       </c>
-      <c r="G3" s="82"/>
+      <c r="G3" s="84"/>
       <c r="H3" s="58"/>
       <c r="I3" s="38"/>
       <c r="J3" s="14"/>
@@ -2699,10 +2703,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="90" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="89"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="5"/>
       <c r="F4" s="37" t="s">
         <v>55</v>
@@ -2731,10 +2735,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="92" t="s">
         <v>189</v>
       </c>
-      <c r="D5" s="91"/>
+      <c r="D5" s="93"/>
       <c r="E5" s="5"/>
       <c r="F5" s="37" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2816,12 +2820,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="83" t="s">
+      <c r="F8" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="85"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="87"/>
       <c r="J8" s="16"/>
       <c r="K8" s="11"/>
       <c r="M8" s="2" t="str">
@@ -2890,7 +2894,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E10" s="63" t="s">
         <v>153</v>
@@ -2914,7 +2918,9 @@
       <c r="J10" s="63" t="s">
         <v>193</v>
       </c>
-      <c r="K10" s="64"/>
+      <c r="K10" s="64" t="s">
+        <v>220</v>
+      </c>
       <c r="O10" s="2" t="str">
         <f>'Definición técnica de imagenes'!A12</f>
         <v>M12D</v>
@@ -2958,7 +2964,7 @@
         <v>195</v>
       </c>
       <c r="K11" s="65" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="O11" s="2" t="str">
         <f>'Definición técnica de imagenes'!A13</f>
@@ -2971,7 +2977,7 @@
         <v>IMG03</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3000,10 +3006,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J12" s="64" t="s">
+        <v>198</v>
+      </c>
+      <c r="K12" s="64" t="s">
         <v>199</v>
-      </c>
-      <c r="K12" s="64" t="s">
-        <v>200</v>
       </c>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>
@@ -3016,7 +3022,7 @@
         <v>IMG04</v>
       </c>
       <c r="B13" s="62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3045,10 +3051,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K13" s="64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
@@ -3061,7 +3067,7 @@
         <v>IMG05</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3090,21 +3096,23 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="64" t="s">
-        <v>205</v>
-      </c>
-      <c r="K14" s="64"/>
+        <v>221</v>
+      </c>
+      <c r="K14" s="64" t="s">
+        <v>222</v>
+      </c>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="202.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="189" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3133,23 +3141,23 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K15" s="66" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3178,10 +3186,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="67" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="K16" s="68" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
@@ -3194,7 +3202,7 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3223,10 +3231,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K17" s="66" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
@@ -3239,7 +3247,7 @@
         <v>IMG09</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3268,10 +3276,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J18" s="66" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K18" s="66" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
@@ -3283,8 +3291,8 @@
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v>IMG10</v>
       </c>
-      <c r="B19" s="110" t="s">
-        <v>216</v>
+      <c r="B19" s="79" t="s">
+        <v>213</v>
       </c>
       <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3313,10 +3321,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="67" t="s">
-        <v>217</v>
-      </c>
-      <c r="K19" s="111" t="s">
-        <v>218</v>
+        <v>214</v>
+      </c>
+      <c r="K19" s="80" t="s">
+        <v>215</v>
       </c>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>
@@ -3329,7 +3337,7 @@
         <v>IMG11</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C20" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3358,10 +3366,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J20" s="64" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K20" s="66" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O20" s="2" t="str">
         <f>'Definición técnica de imagenes'!A32</f>
@@ -6186,25 +6194,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="96"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31"/>
-      <c r="C2" s="97" t="s">
+      <c r="C2" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="98"/>
-      <c r="E2" s="99"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -6212,11 +6220,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="104"/>
-      <c r="E3" s="105"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="107"/>
       <c r="F3" s="32"/>
       <c r="H3" s="22" t="s">
         <v>18</v>
@@ -6267,11 +6275,11 @@
       <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="106" t="str">
+      <c r="D5" s="108" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="107"/>
+      <c r="E5" s="109"/>
       <c r="F5" s="32"/>
       <c r="H5" s="22" t="s">
         <v>22</v>
@@ -6316,12 +6324,12 @@
       <c r="C7" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="92" t="str">
+      <c r="D7" s="94" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="93"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="95"/>
       <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
@@ -6415,14 +6423,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="94" t="s">
+      <c r="A13" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="96"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="98"/>
       <c r="I13" s="22" t="s">
         <v>33</v>
       </c>
@@ -6455,12 +6463,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="97" t="s">
+      <c r="C15" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="99"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="101"/>
       <c r="J15" s="22">
         <v>12</v>
       </c>
@@ -6500,12 +6508,12 @@
       <c r="C17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="100" t="str">
+      <c r="D17" s="102" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="101"/>
-      <c r="F17" s="102"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="104"/>
       <c r="J17" s="22">
         <v>14</v>
       </c>
@@ -6521,12 +6529,12 @@
       <c r="C18" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="92" t="str">
+      <c r="D18" s="94" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="92"/>
-      <c r="F18" s="93"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="95"/>
       <c r="J18" s="22">
         <v>15</v>
       </c>
@@ -6917,40 +6925,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="109" t="s">
+      <c r="B1" s="111" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="109" t="s">
+      <c r="C1" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="109" t="s">
+      <c r="D1" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="109" t="s">
+      <c r="E1" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="109" t="s">
+      <c r="F1" s="111" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="109" t="s">
+      <c r="G1" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="108" t="s">
+      <c r="H1" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="108"/>
+      <c r="I1" s="110"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="109"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
       <c r="H2" s="39" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Eliminación de imagen de Wikipedia
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/SolicitudGrafica CN_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/SolicitudGrafica CN_09_01_CO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="224">
   <si>
     <t>Fecha:</t>
   </si>
@@ -597,15 +597,9 @@
     <t>CN_09_01_CO</t>
   </si>
   <si>
-    <t xml:space="preserve">https://en.wikipedia.org/wiki/DNA#/media/File:Maclyn_McCarty_with_Francis_Crick_and_James_D_Watson_-_10.1371_journal.pbio.0030341.g001-O.jpg </t>
-  </si>
-  <si>
     <t>Ilustración</t>
   </si>
   <si>
-    <t>Foto de James Watson y Francis Crick</t>
-  </si>
-  <si>
     <t xml:space="preserve">http://cuentos-cuanticos.com/2012/05/09/la-expresion-genica-vista-por-un-fisico-i/ </t>
   </si>
   <si>
@@ -684,9 +678,6 @@
     <t>La imagen es para ilustrar. Eliminar de la imagen los textos que se encuentran en color rojo. Escribir los demás nombres en español, así: replicación (ADN – ADN), ADN, transcripción (ADN -&gt; ARN), ARN, traducción (ARN -&gt; Proteína), Proteína</t>
   </si>
   <si>
-    <t>Si entiendo bien, esta imagen requiere que se cite. ¿Nos sirve? No se consiguen fotos sin esas exigencias: si no se puede usar, habrá que eliminarla.</t>
-  </si>
-  <si>
     <t>Comparación del ARN con el ADN</t>
   </si>
   <si>
@@ -700,6 +691,9 @@
   </si>
   <si>
     <t>Ilustrar. Eliminar el recuadro verde que aparece en la parte superior de la imagen, y todo su contenido.</t>
+  </si>
+  <si>
+    <t>Fotografía de un edificio en la universidad de Cambridge</t>
   </si>
 </sst>
 </file>
@@ -2593,9 +2587,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2881,20 +2875,20 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>191</v>
+      <c r="B10" s="62">
+        <v>88447675</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E10" s="63" t="s">
         <v>153</v>
@@ -2916,11 +2910,9 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J10" s="63" t="s">
-        <v>193</v>
-      </c>
-      <c r="K10" s="64" t="s">
-        <v>220</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="K10" s="64"/>
       <c r="O10" s="2" t="str">
         <f>'Definición técnica de imagenes'!A12</f>
         <v>M12D</v>
@@ -2932,14 +2924,14 @@
         <v>IMG02</v>
       </c>
       <c r="B11" s="78" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E11" s="63" t="s">
         <v>153</v>
@@ -2961,10 +2953,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J11" s="64" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K11" s="65" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O11" s="2" t="str">
         <f>'Definición técnica de imagenes'!A13</f>
@@ -2977,14 +2969,14 @@
         <v>IMG03</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E12" s="63" t="s">
         <v>153</v>
@@ -3006,10 +2998,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J12" s="64" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K12" s="64" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>
@@ -3022,14 +3014,14 @@
         <v>IMG04</v>
       </c>
       <c r="B13" s="62" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E13" s="63" t="s">
         <v>153</v>
@@ -3051,10 +3043,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="64" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K13" s="64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
@@ -3067,14 +3059,14 @@
         <v>IMG05</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E14" s="63" t="s">
         <v>153</v>
@@ -3096,10 +3088,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="64" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K14" s="64" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
@@ -3112,14 +3104,14 @@
         <v>IMG06</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" s="63" t="s">
         <v>153</v>
@@ -3141,10 +3133,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K15" s="66" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
@@ -3157,14 +3149,14 @@
         <v>IMG07</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D16" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E16" s="63" t="s">
         <v>153</v>
@@ -3186,10 +3178,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="67" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="K16" s="68" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
@@ -3202,14 +3194,14 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E17" s="63" t="s">
         <v>153</v>
@@ -3231,10 +3223,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K17" s="66" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
@@ -3247,14 +3239,14 @@
         <v>IMG09</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E18" s="63" t="s">
         <v>153</v>
@@ -3276,10 +3268,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J18" s="66" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K18" s="66" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
@@ -3292,14 +3284,14 @@
         <v>IMG10</v>
       </c>
       <c r="B19" s="79" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E19" s="63" t="s">
         <v>153</v>
@@ -3321,10 +3313,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="67" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K19" s="80" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>
@@ -3337,14 +3329,14 @@
         <v>IMG11</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D20" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E20" s="63" t="s">
         <v>153</v>
@@ -3366,10 +3358,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J20" s="64" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K20" s="66" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O20" s="2" t="str">
         <f>'Definición técnica de imagenes'!A32</f>

</xml_diff>